<commit_message>
Updates to 95 citations
</commit_message>
<xml_diff>
--- a/ProcessedData/SCICONF CAandL (R1).xlsx
+++ b/ProcessedData/SCICONF CAandL (R1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\RG Citation Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\RG Citations\rgciting\ProcessedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9FB8EE20-CF9D-42EF-8228-3903DBD1E71B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEFFE8B8-886E-4BB3-B144-B70B85912FA4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="106">
   <si>
     <t>Title</t>
   </si>
@@ -84,9 +84,6 @@
     <t>A014</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>A015</t>
   </si>
   <si>
@@ -192,49 +189,160 @@
     <t>A045</t>
   </si>
   <si>
+    <t>A046</t>
+  </si>
+  <si>
+    <t>A047</t>
+  </si>
+  <si>
+    <t>A048</t>
+  </si>
+  <si>
+    <t>A049</t>
+  </si>
+  <si>
+    <t>A050</t>
+  </si>
+  <si>
+    <t>A051</t>
+  </si>
+  <si>
+    <t>A052</t>
+  </si>
+  <si>
+    <t>A053</t>
+  </si>
+  <si>
+    <t>A054</t>
+  </si>
+  <si>
+    <t>A055</t>
+  </si>
+  <si>
+    <t>A056</t>
+  </si>
+  <si>
+    <t>A057</t>
+  </si>
+  <si>
+    <t>A058</t>
+  </si>
+  <si>
+    <t>A059</t>
+  </si>
+  <si>
+    <t>A061</t>
+  </si>
+  <si>
+    <t>A062</t>
+  </si>
+  <si>
+    <t>A063</t>
+  </si>
+  <si>
+    <t>A064</t>
+  </si>
+  <si>
+    <t>A065</t>
+  </si>
+  <si>
+    <t>A066</t>
+  </si>
+  <si>
+    <t>A067</t>
+  </si>
+  <si>
+    <t>A068</t>
+  </si>
+  <si>
+    <t>A069</t>
+  </si>
+  <si>
+    <t>A070</t>
+  </si>
+  <si>
+    <t>A071</t>
+  </si>
+  <si>
+    <t>A072</t>
+  </si>
+  <si>
+    <t>A060</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>A073</t>
+  </si>
+  <si>
+    <t>A074</t>
+  </si>
+  <si>
+    <t>A075</t>
+  </si>
+  <si>
+    <t>A076</t>
+  </si>
+  <si>
+    <t>A077</t>
+  </si>
+  <si>
+    <t>A078</t>
+  </si>
+  <si>
+    <t>A079</t>
+  </si>
+  <si>
+    <t>A080</t>
+  </si>
+  <si>
+    <t>A081</t>
+  </si>
+  <si>
+    <t>A082</t>
+  </si>
+  <si>
+    <t>A083</t>
+  </si>
+  <si>
     <t>None</t>
   </si>
   <si>
-    <t>A046</t>
-  </si>
-  <si>
-    <t>A047</t>
-  </si>
-  <si>
-    <t>A048</t>
-  </si>
-  <si>
-    <t>A049</t>
-  </si>
-  <si>
-    <t>A050</t>
-  </si>
-  <si>
-    <t>A051</t>
-  </si>
-  <si>
-    <t>A052</t>
-  </si>
-  <si>
-    <t>A053</t>
-  </si>
-  <si>
-    <t>A054</t>
-  </si>
-  <si>
-    <t>A055</t>
-  </si>
-  <si>
-    <t>A056</t>
-  </si>
-  <si>
-    <t>A057</t>
-  </si>
-  <si>
-    <t>A058</t>
-  </si>
-  <si>
-    <t>A059</t>
+    <t>A092</t>
+  </si>
+  <si>
+    <t>A084</t>
+  </si>
+  <si>
+    <t>A085</t>
+  </si>
+  <si>
+    <t>A086</t>
+  </si>
+  <si>
+    <t>A087</t>
+  </si>
+  <si>
+    <t>A088</t>
+  </si>
+  <si>
+    <t>A089</t>
+  </si>
+  <si>
+    <t>A090</t>
+  </si>
+  <si>
+    <t>A091</t>
+  </si>
+  <si>
+    <t>A093</t>
+  </si>
+  <si>
+    <t>A094</t>
+  </si>
+  <si>
+    <t>A095</t>
   </si>
 </sst>
 </file>
@@ -597,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,10 +883,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -786,10 +894,10 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
         <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -800,7 +908,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -811,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -822,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -833,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -844,7 +952,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -855,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -866,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -877,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -888,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -899,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -910,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -921,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -932,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -943,18 +1051,18 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -965,29 +1073,29 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
         <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -998,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1009,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1020,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1031,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1042,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1053,7 +1161,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1064,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1075,18 +1183,18 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1097,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1108,74 +1216,74 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>53</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1186,7 +1294,7 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1197,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1208,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1219,7 +1327,7 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1230,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1241,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1252,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1263,18 +1371,18 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1285,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1296,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1307,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1318,7 +1426,776 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" t="s">
+        <v>39</v>
+      </c>
+      <c r="C68" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>81</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>81</v>
+      </c>
+      <c r="C110" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>81</v>
+      </c>
+      <c r="C111" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>81</v>
+      </c>
+      <c r="C114" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>81</v>
+      </c>
+      <c r="C115" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>81</v>
+      </c>
+      <c r="C119" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>81</v>
+      </c>
+      <c r="C120" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>81</v>
+      </c>
+      <c r="C121" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>81</v>
+      </c>
+      <c r="C122" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>81</v>
+      </c>
+      <c r="C123" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>81</v>
+      </c>
+      <c r="C124" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>81</v>
+      </c>
+      <c r="C125" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>81</v>
+      </c>
+      <c r="C126" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>81</v>
+      </c>
+      <c r="C127" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>81</v>
+      </c>
+      <c r="C128" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>93</v>
+      </c>
+      <c r="C129" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>81</v>
+      </c>
+      <c r="C130" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>81</v>
+      </c>
+      <c r="C131" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>81</v>
+      </c>
+      <c r="C132" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>0</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>4</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>36</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>0</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>0</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>